<commit_message>
inspector update and camera features
</commit_message>
<xml_diff>
--- a/script/dialogues.xlsx
+++ b/script/dialogues.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">test1</t>
   </si>
   <si>
-    <t xml:space="preserve">[ ["SAY" ,{"name": "dahlia", "mood": "happy"}],["SAY" ,{"name": "dahlia", "mood": "thinking"}] ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">["#dialog_set_speed;5##dialog_set_track;dahlia#Hello everyone :D this is a long text that will likely overflow of this message box, spilling it’s contents outside and litter the universe..","This is a nice day"]</t>
+    <t xml:space="preserve">[ ["SAY" ,{"name": "dahlia", "mood": "happy"}], ["SAY" ,{"name": "dahlia", "mood": "happy"}], ["SAY" ,{"name": "dahlia", "mood": "thinking"}], ["SAY" ,{"name": "dahlia", "mood": "happy"}] ,["SAY",{"name":"???"}]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["#set_speed;5##set_track;dahlia#Hello everyone :D this is a long text that will likely overflow of this message box, spilling it’s contents outside and litter the universe.","#set_speed;4#However as you can see, this panel is adapting to fit everything :D even with long-ass words, watch : thisisaverylongwordandidon’tknowwhattowritetomakeitlongerhopefullyyougetitbynowherehavesomegibberishforgoodmeasuregbnhirltuhgtbiuthvbiliu","hmmm…","Nice weather we’re having today, isn’t it ?","#set_speed;0.2#yeah it’s nice.#set_delay;1000#"]</t>
   </si>
   <si>
     <t xml:space="preserve">test2</t>
@@ -161,10 +161,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.31"/>
@@ -182,7 +182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="99.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
smooth selection frame + dialog panel resize
</commit_message>
<xml_diff>
--- a/script/dialogues.xlsx
+++ b/script/dialogues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">TEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Croatian</t>
   </si>
   <si>
     <t xml:space="preserve">test1</t>
@@ -158,13 +164,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.31"/>
@@ -181,38 +187,44 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="99.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="122.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>